<commit_message>
finished schematic and layout checklists. passed DRC
</commit_message>
<xml_diff>
--- a/1 Hardware/MCP33151 Eval Board/MCP33151 Eval Board Schematic Symbol and Footprint Checks.xlsx
+++ b/1 Hardware/MCP33151 Eval Board/MCP33151 Eval Board Schematic Symbol and Footprint Checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\1 Hardware\MCP33151 Eval Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCA6E6E-C535-4ECB-988F-CB6671104F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A081BD47-5C63-410A-A4B7-1C672B4D41B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="1" xr2:uid="{32DD5F8E-229B-48BF-858D-EACE20E5D4CD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{32DD5F8E-229B-48BF-858D-EACE20E5D4CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>Component</t>
   </si>
@@ -176,11 +176,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,23 +272,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>111182</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>493608</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>20955</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E5FDBA-A8B5-4BF9-9FC1-7B328A25B47D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9A1C9A-5A1B-7C72-68C3-95F0E4982263}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -308,13 +311,216 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7563542" y="114300"/>
-          <a:ext cx="2319598" cy="4488180"/>
+          <a:off x="8132658" y="163830"/>
+          <a:ext cx="3188757" cy="4956810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>265721</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>89203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>103534</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE6AFA21-1B3F-7024-679D-6276DB5C6DF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11737134" y="89203"/>
+          <a:ext cx="2902378" cy="3033340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>150494</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>264171</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2121D03A-A5B0-BB31-7162-A14AF82C6878}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11706226" y="3227069"/>
+          <a:ext cx="3045470" cy="3307080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>781834</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>130660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>529140</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BBF18E3-40B2-009A-E58C-E4E55776212F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7326069" y="5330189"/>
+          <a:ext cx="4016747" cy="3918585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -850,15 +1056,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A94FF0-21C5-447E-ADFF-8779BFE992A7}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -884,11 +1090,26 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
@@ -899,6 +1120,9 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -907,6 +1131,9 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -915,6 +1142,9 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -923,6 +1153,9 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -931,26 +1164,86 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -959,26 +1252,75 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -998,8 +1340,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="C3:E7"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>